<commit_message>
do a lot =)
</commit_message>
<xml_diff>
--- a/handlers/materials_for_studying/task_1/task_1.xlsx
+++ b/handlers/materials_for_studying/task_1/task_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\easyegerussian_bot\handlers\materials_for_studying\task_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\win_ubuntu\telegram_bot\handlers\materials_for_studying\task_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CBD67C-A88D-4B7D-85B5-4DDFCCB0BEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7104F97-5965-4626-A3FD-88A2830F0CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -427,24 +427,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.73046875" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
-    <col min="4" max="4" width="44.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.1328125" customWidth="1"/>
+    <col min="4" max="4" width="44.1328125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.73046875" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -470,7 +470,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -482,6 +482,36 @@
       </c>
       <c r="D2" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>